<commit_message>
[GEN MCU] Reset IC review data update
</commit_message>
<xml_diff>
--- a/1_LF_Generator_MCU/4_Review Data/Plasma_LF_GEN_MCU_Review data.xlsx
+++ b/1_LF_Generator_MCU/4_Review Data/Plasma_LF_GEN_MCU_Review data.xlsx
@@ -4,20 +4,64 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Reset IC" sheetId="1" r:id="rId1"/>
     <sheet name="LED control" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>Vcc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/RESET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reset IC operation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VDD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VIH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VIL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MCU NRST Voltage detection threshold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NRST의 High level이 1.87이므로 /RESET 2.7V도 High로 인식한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>23ㅛㅓ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -32,16 +76,31 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -49,12 +108,202 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -67,6 +316,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>153536</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>171995</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="그림 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5753100" y="295275"/>
+          <a:ext cx="8135486" cy="3905795"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -356,16 +648,140 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="4.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="13">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C4" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="14">
+        <f>D3*0.445+0.398</f>
+        <v>1.8664999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="15">
+        <f>D3*0.3+0.07</f>
+        <v>1.0599999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C9" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="D9" s="2">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C10" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="D10" s="4">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C11" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="D11" s="4">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C12" s="3">
+        <v>3</v>
+      </c>
+      <c r="D12" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C13" s="3">
+        <v>2.9</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C14" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C15" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="5">
+        <v>2.6</v>
+      </c>
+      <c r="D16" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="I28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -373,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>